<commit_message>
hist worksheet 1 started and grades update
</commit_message>
<xml_diff>
--- a/2.1-HIST-1302.005/Grades.xlsx
+++ b/2.1-HIST-1302.005/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\2.1-HIST-1302.005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0976C7A1-848F-444C-A58C-C514F3DD08F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEC0E51-1FA2-4666-9DF7-BD383B33FE76}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4830" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,7 +673,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>0.18049999999999999</v>
+        <v>0.18240000000000001</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
@@ -816,7 +816,7 @@
       <c r="I7" s="22"/>
       <c r="J7" s="22">
         <f>SUM(C7:H7)</f>
-        <v>1.0455000000000001</v>
+        <v>1.0474000000000001</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="5"/>
@@ -832,7 +832,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="21">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
HIST exam 1 grade
</commit_message>
<xml_diff>
--- a/2.1-HIST-1302.005/Grades.xlsx
+++ b/2.1-HIST-1302.005/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\2.1-HIST-1302.005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163F1B2-21C9-4B97-B9BF-2C18947A7B22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAC768F-4C78-4DD3-AA78-E29E82D17408}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1680" windowWidth="16290" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="2580" windowWidth="21165" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +807,7 @@
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
-        <v>0.61499999999999999</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="1"/>
@@ -816,7 +816,7 @@
       <c r="I7" s="22"/>
       <c r="J7" s="22">
         <f>SUM(C7:H7)</f>
-        <v>1.0398000000000001</v>
+        <v>0.99879999999999991</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="5"/>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="10">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="22"/>

</xml_diff>

<commit_message>
worksheet 2 final download. Doc 7 started. Grades(Blank) created
</commit_message>
<xml_diff>
--- a/2.1-HIST-1302.005/Grades.xlsx
+++ b/2.1-HIST-1302.005/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\2.1-HIST-1302.005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAC768F-4C78-4DD3-AA78-E29E82D17408}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387197B4-187E-4486-B9CC-9DC76E56B062}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="2580" windowWidth="21165" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="1950" windowWidth="24345" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,23 +253,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,12 +310,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -673,7 +661,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,413 +673,413 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22" t="s">
+      <c r="H4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>0</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <v>0.19</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>0.06</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>0.19</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="10">
         <v>0.61499999999999999</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <v>0</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
         <f>SUM(C5:H5)</f>
         <v>1.0549999999999999</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="2" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <f t="shared" ref="C6:H6" si="0">COUNT(C8:C21)</f>
         <v>4</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <f t="shared" ref="C7:H7" si="1">IF(C6&lt;&gt;0,IF(C5&lt;&gt;0,(SUM(C8:C21)/C6)*C5,0), 0)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <f t="shared" si="1"/>
         <v>0.17479999999999998</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="H7" s="9">
+        <v>0.51454999999999995</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
         <f>SUM(C7:H7)</f>
-        <v>0.99879999999999991</v>
-      </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="5"/>
+        <v>0.93934999999999991</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="19">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="17">
         <v>0.5</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="19">
         <v>0.6</v>
       </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10">
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
         <v>0.8</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="2"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18">
-        <v>1</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="12">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="2"/>
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="20">
-        <v>1</v>
-      </c>
-      <c r="D10" s="18">
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
         <v>0.6</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="12">
-        <v>1</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="2"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="20">
-        <v>1</v>
-      </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="2"/>
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>5</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="18">
-        <v>1</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="2"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>6</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="18">
-        <v>1</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="2"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>7</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="18">
-        <v>1</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="2"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>8</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="18">
-        <v>1</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="2"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>9</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="18">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="2"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="18">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="2"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>11</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="2"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>12</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="2"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>13</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="2"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
     </row>
     <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>14</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="2"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>